<commit_message>
Updates button component name
</commit_message>
<xml_diff>
--- a/Angular Udemy Course.xlsx
+++ b/Angular Udemy Course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keith.tomlinson/Documents/AngularCourse/AngularUdemyExercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEE1DE3A-2195-E947-8107-08D3C2275636}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77133C10-F149-604D-B8A9-CA0BFE3316CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="-20260" windowWidth="28040" windowHeight="17440" xr2:uid="{9F894929-3D12-6A4F-9CBC-F6861D3954DE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{9F894929-3D12-6A4F-9CBC-F6861D3954DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="597">
   <si>
     <t>ANGULAR</t>
   </si>
@@ -2199,7 +2199,7 @@
   <dimension ref="A1:B1134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2350,133 +2350,181 @@
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B22" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="B23" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="B24" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B25" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="B26" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="B27" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="B28" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="B29" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="B30" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="B31" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>52</v>
       </c>
@@ -2627,7 +2675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>12</v>
       </c>

</xml_diff>